<commit_message>
Recollected Jfreechart and Jodatime results and updated Results.xlsx
</commit_message>
<xml_diff>
--- a/results/Results.xlsx
+++ b/results/Results.xlsx
@@ -486,6 +486,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -515,48 +557,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -848,7 +848,7 @@
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="43" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -867,151 +867,151 @@
   <sheetData>
     <row r="1" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="37"/>
-    </row>
-    <row r="2" spans="1:36" s="57" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="54" t="s">
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="50"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="51"/>
+    </row>
+    <row r="2" spans="1:36" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="55" t="s">
+      <c r="K2" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="L2" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="55" t="s">
+      <c r="M2" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="55" t="s">
+      <c r="N2" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="55" t="s">
+      <c r="O2" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="55" t="s">
+      <c r="P2" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="56" t="s">
+      <c r="Q2" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="56" t="s">
+      <c r="R2" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="56" t="s">
+      <c r="S2" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="56" t="s">
+      <c r="T2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="56" t="s">
+      <c r="U2" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="56" t="s">
+      <c r="V2" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="56" t="s">
+      <c r="W2" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="56" t="s">
+      <c r="X2" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="56" t="s">
+      <c r="Y2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="56" t="s">
+      <c r="Z2" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" s="56" t="s">
+      <c r="AA2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AB2" s="56" t="s">
+      <c r="AB2" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="AC2" s="56" t="s">
+      <c r="AC2" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="AD2" s="56" t="s">
+      <c r="AD2" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AE2" s="56" t="s">
+      <c r="AE2" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AF2" s="56" t="s">
+      <c r="AF2" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AG2" s="56" t="s">
+      <c r="AG2" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="AH2" s="56" t="s">
+      <c r="AH2" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AI2" s="56" t="s">
+      <c r="AI2" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="AJ2" s="56" t="s">
+      <c r="AJ2" s="46" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1022,7 +1022,7 @@
       <c r="B3" s="17">
         <v>0</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="38">
         <v>0</v>
       </c>
       <c r="D3" s="17">
@@ -1132,7 +1132,7 @@
       <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="37">
         <v>3</v>
       </c>
       <c r="D4" s="11">
@@ -1242,7 +1242,7 @@
       <c r="B5" s="8">
         <v>22</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="37">
         <v>48</v>
       </c>
       <c r="D5" s="11">
@@ -1462,7 +1462,7 @@
       <c r="B7" s="8">
         <v>66</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="37">
         <v>78</v>
       </c>
       <c r="D7" s="11">
@@ -1568,7 +1568,7 @@
     <row r="8" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="49"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -1585,151 +1585,151 @@
     </row>
     <row r="9" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="36"/>
-      <c r="S9" s="36"/>
-      <c r="T9" s="36"/>
-      <c r="U9" s="36"/>
-      <c r="V9" s="36"/>
-      <c r="W9" s="36"/>
-      <c r="X9" s="36"/>
-      <c r="Y9" s="36"/>
-      <c r="Z9" s="36"/>
-      <c r="AA9" s="36"/>
-      <c r="AB9" s="36"/>
-      <c r="AC9" s="36"/>
-      <c r="AD9" s="36"/>
-      <c r="AE9" s="36"/>
-      <c r="AF9" s="36"/>
-      <c r="AG9" s="36"/>
-      <c r="AH9" s="36"/>
-      <c r="AI9" s="36"/>
-      <c r="AJ9" s="37"/>
-    </row>
-    <row r="10" spans="1:36" s="57" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="54" t="s">
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
+      <c r="O9" s="50"/>
+      <c r="P9" s="50"/>
+      <c r="Q9" s="50"/>
+      <c r="R9" s="50"/>
+      <c r="S9" s="50"/>
+      <c r="T9" s="50"/>
+      <c r="U9" s="50"/>
+      <c r="V9" s="50"/>
+      <c r="W9" s="50"/>
+      <c r="X9" s="50"/>
+      <c r="Y9" s="50"/>
+      <c r="Z9" s="50"/>
+      <c r="AA9" s="50"/>
+      <c r="AB9" s="50"/>
+      <c r="AC9" s="50"/>
+      <c r="AD9" s="50"/>
+      <c r="AE9" s="50"/>
+      <c r="AF9" s="50"/>
+      <c r="AG9" s="50"/>
+      <c r="AH9" s="50"/>
+      <c r="AI9" s="50"/>
+      <c r="AJ9" s="51"/>
+    </row>
+    <row r="10" spans="1:36" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="44" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="55" t="s">
+      <c r="D10" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="55" t="s">
+      <c r="E10" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="55" t="s">
+      <c r="F10" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="55" t="s">
+      <c r="G10" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="55" t="s">
+      <c r="H10" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="55" t="s">
+      <c r="I10" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="55" t="s">
+      <c r="J10" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="55" t="s">
+      <c r="K10" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="55" t="s">
+      <c r="L10" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="55" t="s">
+      <c r="M10" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="55" t="s">
+      <c r="N10" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="55" t="s">
+      <c r="O10" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="P10" s="55" t="s">
+      <c r="P10" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="56" t="s">
+      <c r="Q10" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="R10" s="56" t="s">
+      <c r="R10" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="S10" s="56" t="s">
+      <c r="S10" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="T10" s="56" t="s">
+      <c r="T10" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="U10" s="56" t="s">
+      <c r="U10" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="V10" s="56" t="s">
+      <c r="V10" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="W10" s="56" t="s">
+      <c r="W10" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="X10" s="56" t="s">
+      <c r="X10" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="Y10" s="56" t="s">
+      <c r="Y10" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="Z10" s="56" t="s">
+      <c r="Z10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="AA10" s="56" t="s">
+      <c r="AA10" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AB10" s="56" t="s">
+      <c r="AB10" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="AC10" s="56" t="s">
+      <c r="AC10" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="AD10" s="56" t="s">
+      <c r="AD10" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="AE10" s="56" t="s">
+      <c r="AE10" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AF10" s="56" t="s">
+      <c r="AF10" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AG10" s="56" t="s">
+      <c r="AG10" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="AH10" s="56" t="s">
+      <c r="AH10" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AI10" s="56" t="s">
+      <c r="AI10" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="AJ10" s="56" t="s">
+      <c r="AJ10" s="46" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1740,7 +1740,7 @@
       <c r="B11" s="16">
         <v>8</v>
       </c>
-      <c r="C11" s="50">
+      <c r="C11" s="40">
         <v>8</v>
       </c>
       <c r="D11" s="13">
@@ -1850,7 +1850,7 @@
       <c r="B12" s="8">
         <v>0</v>
       </c>
-      <c r="C12" s="47">
+      <c r="C12" s="37">
         <v>0</v>
       </c>
       <c r="D12" s="11">
@@ -1960,7 +1960,7 @@
       <c r="B13" s="8">
         <v>0</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="37">
         <v>0</v>
       </c>
       <c r="D13" s="11">
@@ -2286,7 +2286,7 @@
     <row r="16" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="51"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
@@ -2304,7 +2304,7 @@
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="51"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -2322,7 +2322,7 @@
     <row r="18" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
-      <c r="C18" s="52"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
@@ -2368,13 +2368,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27"/>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="55"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
@@ -2506,13 +2506,13 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27"/>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
@@ -2694,9 +2694,9 @@
       <c r="A23" s="18"/>
     </row>
     <row r="24" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
+      <c r="A24" s="52"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
@@ -2743,7 +2743,7 @@
   <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2759,16 +2759,16 @@
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26"/>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="44"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="58"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -2806,7 +2806,7 @@
       <c r="B3" s="33">
         <v>0</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="35">
         <v>0</v>
       </c>
       <c r="D3" s="33">
@@ -2835,7 +2835,7 @@
       <c r="B4" s="12">
         <v>64</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="36">
         <v>66</v>
       </c>
       <c r="D4" s="12">
@@ -2864,7 +2864,7 @@
       <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="37">
         <v>0</v>
       </c>
       <c r="D5" s="12">
@@ -2893,7 +2893,7 @@
       <c r="B6" s="5">
         <v>24</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="37">
         <v>30</v>
       </c>
       <c r="D6" s="12">
@@ -2929,16 +2929,16 @@
     </row>
     <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26"/>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="44"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="58"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
@@ -2973,27 +2973,59 @@
       <c r="A11" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="B11" s="33">
+        <v>0</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>0</v>
+      </c>
+      <c r="G11" s="33">
+        <v>0</v>
+      </c>
+      <c r="H11" s="33">
+        <v>0</v>
+      </c>
+      <c r="I11" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="B12" s="12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>1</v>
+      </c>
+      <c r="I12" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -3002,7 +3034,7 @@
       <c r="B13" s="5">
         <v>0</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="37">
         <v>0</v>
       </c>
       <c r="D13" s="12">
@@ -3031,7 +3063,7 @@
       <c r="B14" s="5">
         <v>0</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="37">
         <v>0</v>
       </c>
       <c r="D14" s="12">

</xml_diff>